<commit_message>
add new utils and Integration
</commit_message>
<xml_diff>
--- a/ExcelReport.xlsx
+++ b/ExcelReport.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="82">
   <si>
     <t>id</t>
   </si>
@@ -43,7 +43,7 @@
     <t>failure</t>
   </si>
   <si>
-    <t>c31466ac-2b02-4406-b02a-2ee24c9dafc6</t>
+    <t>e505472b-6a2f-4966-8ba1-2e5e4f0ce5f0</t>
   </si>
   <si>
     <t>WebDriver University Functionality</t>
@@ -55,10 +55,13 @@
     <t>src/tests/features/webDriverUniversity.feature</t>
   </si>
   <si>
-    <t>[]</t>
-  </si>
-  <si>
-    <t>["the user opens the CONTACT US form","the user enters valid information","the form is submitted successfully"]</t>
+    <t xml:space="preserve">@Regression
+@ContactForm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user opens the CONTACT US form
+the user enters valid information
+the form is submitted successfully</t>
   </si>
   <si>
     <t>PENDING</t>
@@ -67,148 +70,244 @@
     <t/>
   </si>
   <si>
-    <t>956fefbb-c127-4b76-868c-a98218ed0491</t>
+    <t>82259def-5c08-46a9-a723-9b78b3faba69</t>
   </si>
   <si>
     <t>LOGIN PORTAL</t>
   </si>
   <si>
-    <t>["the user navigates to the LOGIN PORTAL","the user enters valid username and password","access is granted"]</t>
-  </si>
-  <si>
-    <t>854c4c6a-966e-414a-a363-3bc00b5e0746</t>
+    <t xml:space="preserve">@Regression
+@LoginPortal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user navigates to the LOGIN PORTAL
+the user enters valid username and password
+access is granted</t>
+  </si>
+  <si>
+    <t>19dac02c-72cc-419a-9718-e96ca982d59b</t>
   </si>
   <si>
     <t>BUTTON CLICKS</t>
   </si>
   <si>
-    <t>["the user is on the BUTTON CLICKS page","the user performs all types of clicks","all clicks are registered successfully"]</t>
-  </si>
-  <si>
-    <t>77c4145f-b2fd-43dc-a81f-621a1a29c43f</t>
+    <t xml:space="preserve">@Regression
+@ButtonClicks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user is on the BUTTON CLICKS page
+the user performs all types of clicks
+all clicks are registered successfully</t>
+  </si>
+  <si>
+    <t>ff85650b-91a1-4f8b-96f8-dbe1183bb98d</t>
   </si>
   <si>
     <t>TO DO LIST</t>
   </si>
   <si>
-    <t>["the user has a list of tasks","the user adds and deletes tasks using Webdriver methods","the list updates correctly"]</t>
-  </si>
-  <si>
-    <t>964ef93b-f831-48f0-b15e-797e085f3591</t>
+    <t xml:space="preserve">@Regression
+@TodoList</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user has a list of tasks
+the user adds and deletes tasks using Webdriver methods
+the list updates correctly</t>
+  </si>
+  <si>
+    <t>f3b4c613-576c-43ad-811e-a1817dfe1f0f</t>
   </si>
   <si>
     <t>PAGE OBJECT MODEL</t>
   </si>
   <si>
-    <t>["the user is familiar with the Page Object Model","the user applies POM concepts to model website pages","the pages are modeled correctly"]</t>
-  </si>
-  <si>
-    <t>4aea073b-7617-4ded-9108-09bd92162f4a</t>
+    <t xml:space="preserve">@Regression
+@PageObjectModel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user is familiar with the Page Object Model
+the user applies POM concepts to model website pages
+the pages are modeled correctly</t>
+  </si>
+  <si>
+    <t>13ab8b26-1d85-4ec3-9eb8-0639d931397a</t>
   </si>
   <si>
     <t>ACCORDION &amp; TEXT AFFECTS</t>
   </si>
   <si>
-    <t>["the user clicks on one of the accordion panels","the user waits for the text to appear","the user sees the text toggling as expected"]</t>
-  </si>
-  <si>
-    <t>f77cd5d5-7888-4801-b8af-8e14d4746eb3</t>
+    <t xml:space="preserve">@Regression
+@AccordionAndTextAffects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user clicks on one of the accordion panels
+the user waits for the text to appear
+the user sees the text toggling as expected</t>
+  </si>
+  <si>
+    <t>1b5848f4-f482-43cd-a66b-ee383a2e106d</t>
   </si>
   <si>
     <t>DROPDOWN, CHECKBOXES &amp; RADIO BUTTONS</t>
   </si>
   <si>
-    <t>["the user is presented with dropdowns, checkboxes, and radio buttons","the user selects different options","the selections are reflected correctly"]</t>
-  </si>
-  <si>
-    <t>36db0c2e-1dde-4895-9df5-fef77edae739</t>
+    <t xml:space="preserve">@Regression
+@Dropdown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user is presented with dropdowns, checkboxes, and radio buttons
+the user selects different options
+the selections are reflected correctly</t>
+  </si>
+  <si>
+    <t>882f736d-e6c6-4912-a341-541461328cb6</t>
   </si>
   <si>
     <t>AJAX LOADER</t>
   </si>
   <si>
-    <t>["the user encounters an Ajax Loader","the user waits for the loader to finish","the user can interact with the elements loaded"]</t>
-  </si>
-  <si>
-    <t>02a215a0-3c80-4958-80f6-a895d2f768ff</t>
+    <t xml:space="preserve">@Regression
+@AjaxLoader</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user encounters an Ajax Loader
+the user waits for the loader to finish
+the user can interact with the elements loaded</t>
+  </si>
+  <si>
+    <t>c247de79-68f7-4bef-914a-d1c44cc05a39</t>
   </si>
   <si>
     <t>ACTIONS</t>
   </si>
   <si>
-    <t>["the user needs to perform complex actions","the user attempts double clicks, clicks and holds, or drags and drops","the actions are performed successfully"]</t>
-  </si>
-  <si>
-    <t>a9ce9f70-b5ed-4449-a177-8f994c2a2d09</t>
+    <t xml:space="preserve">@Regression
+@Actions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user needs to perform complex actions
+the user attempts double clicks, clicks and holds, or drags and drops
+the actions are performed successfully</t>
+  </si>
+  <si>
+    <t>f25202c4-2e53-496c-8304-76ffdbcfe54b</t>
   </si>
   <si>
     <t>SCROLLING AROUND</t>
   </si>
   <si>
-    <t>["the user needs to scroll to a specific element","the user scrolls to that element","the user can interact with it successfully"]</t>
-  </si>
-  <si>
-    <t>b4426fa7-ec38-4b9c-86ec-abc00a57dbc3</t>
+    <t xml:space="preserve">@Regression
+@ScronllingArround</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user needs to scroll to a specific element
+the user scrolls to that element
+the user can interact with it successfully</t>
+  </si>
+  <si>
+    <t>348db6cc-d244-42e8-a717-aaf461b49e6c</t>
   </si>
   <si>
     <t>POPUP &amp; ALERTS</t>
   </si>
   <si>
-    <t>["the user encounters popups and alerts","the user attempts to close or handle them","the popups and alerts are managed successfully"]</t>
-  </si>
-  <si>
-    <t>2aa78817-3a47-4d29-b86c-bb5ff4cb030d</t>
+    <t xml:space="preserve">@Regression
+@PopupAlerts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user encounters popups and alerts
+the user attempts to close or handle them
+the popups and alerts are managed successfully</t>
+  </si>
+  <si>
+    <t>095a7305-b289-4877-a62d-e8997e34b5cd</t>
   </si>
   <si>
     <t>IFRAME</t>
   </si>
   <si>
-    <t>["the user needs to interact with elements within an IFRAME","the user switches context to the IFRAME","the user can interact with the elements within the IFRAME"]</t>
-  </si>
-  <si>
-    <t>414f842e-35d1-498f-943b-28da80322f2d</t>
+    <t xml:space="preserve">@Regression
+@Iframe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user needs to interact with elements within an IFRAME
+the user switches context to the IFRAME
+the user can interact with the elements within the IFRAME</t>
+  </si>
+  <si>
+    <t>439ec24b-3b5e-4000-a033-340aa0dc8142</t>
   </si>
   <si>
     <t>HIDDEN ELEMENTS</t>
   </si>
   <si>
-    <t>["the user suspects the presence of hidden elements","the user inspects and interacts with these elements","the hidden elements are handled correctly"]</t>
-  </si>
-  <si>
-    <t>330ed9c9-d929-42d8-8a80-38c42b6ee384</t>
+    <t xml:space="preserve">@Regression
+@HiddenElements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user suspects the presence of hidden elements
+the user inspects and interacts with these elements
+the hidden elements are handled correctly</t>
+  </si>
+  <si>
+    <t>25317202-9cdf-4367-a7e7-e0de6bd1be72</t>
   </si>
   <si>
     <t>DATA, TABLES &amp; BUTTON STATES</t>
   </si>
   <si>
-    <t>["the user needs to work with data from a table","the user reads and possibly writes data to and from the table","the data is handled correctly"]</t>
-  </si>
-  <si>
-    <t>a6b0ba96-ae34-4190-b8a5-1bfe868a7e31</t>
+    <t xml:space="preserve">@Regression
+@DataTablesButtonStates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user needs to work with data from a table
+the user reads and possibly writes data to and from the table
+the data is handled correctly</t>
+  </si>
+  <si>
+    <t>fbedf1f8-8dec-4f35-abfb-baba615bdea9</t>
   </si>
   <si>
     <t>AUTOCOMPLETE TEXTFIELD</t>
   </si>
   <si>
-    <t>["the user starts typing in the autocomplete text field","the user selects an item from the autocomplete suggestions","the selected item reflects the user's needs"]</t>
-  </si>
-  <si>
-    <t>825922ce-ac7c-4c69-83f7-447b609ffd77</t>
+    <t xml:space="preserve">@Regression
+@AutoCompleteTextField</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user starts typing in the autocomplete text field
+the user selects an item from the autocomplete suggestions
+the selected item reflects the user's needs</t>
+  </si>
+  <si>
+    <t>dd11d7db-3055-4e1e-a77b-51992914619f</t>
   </si>
   <si>
     <t>FILE UPLOAD</t>
   </si>
   <si>
-    <t>["the user has a specific file to upload","the user chooses the file and submits it","the file is uploaded successfully"]</t>
-  </si>
-  <si>
-    <t>ababc773-8c21-4f9c-bf94-c9aca986fc6f</t>
+    <t xml:space="preserve">@Regression
+@FileUpload</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user has a specific file to upload
+the user chooses the file and submits it
+the file is uploaded successfully</t>
+  </si>
+  <si>
+    <t>9dc7ee91-cfe2-4f6f-af6e-94a75f4d5929</t>
   </si>
   <si>
     <t>DATEPICKER</t>
   </si>
   <si>
-    <t>["the user is presented with a datepicker","the user selects a day, month, and year","the selected date is accepted and displayed correctly"]</t>
+    <t xml:space="preserve">@Regression
+@DatePicker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the user is presented with a datepicker
+the user selects a day, month, and year
+the selected date is accepted and displayed correctly</t>
   </si>
 </sst>
 </file>
@@ -643,7 +742,7 @@
         <v>16</v>
       </c>
       <c r="H2">
-        <v>620042</v>
+        <v>560625</v>
       </c>
       <c r="I2" t="b">
         <v>0</v>
@@ -666,16 +765,16 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s">
         <v>16</v>
       </c>
       <c r="H3">
-        <v>503749</v>
+        <v>619000</v>
       </c>
       <c r="I3" t="b">
         <v>0</v>
@@ -686,28 +785,28 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G4" t="s">
         <v>16</v>
       </c>
       <c r="H4">
-        <v>502750</v>
+        <v>534541</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
@@ -718,28 +817,28 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G5" t="s">
         <v>16</v>
       </c>
       <c r="H5">
-        <v>760665</v>
+        <v>891832</v>
       </c>
       <c r="I5" t="b">
         <v>0</v>
@@ -750,28 +849,28 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G6" t="s">
         <v>16</v>
       </c>
       <c r="H6">
-        <v>486124</v>
+        <v>704792</v>
       </c>
       <c r="I6" t="b">
         <v>0</v>
@@ -782,28 +881,28 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="G7" t="s">
         <v>16</v>
       </c>
       <c r="H7">
-        <v>478082</v>
+        <v>726375</v>
       </c>
       <c r="I7" t="b">
         <v>0</v>
@@ -814,28 +913,28 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G8" t="s">
         <v>16</v>
       </c>
       <c r="H8">
-        <v>610083</v>
+        <v>742292</v>
       </c>
       <c r="I8" t="b">
         <v>0</v>
@@ -846,28 +945,28 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="F9" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="G9" t="s">
         <v>16</v>
       </c>
       <c r="H9">
-        <v>781666</v>
+        <v>826167</v>
       </c>
       <c r="I9" t="b">
         <v>0</v>
@@ -878,28 +977,28 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="G10" t="s">
         <v>16</v>
       </c>
       <c r="H10">
-        <v>507959</v>
+        <v>510041</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
@@ -910,28 +1009,28 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>52</v>
       </c>
       <c r="F11" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="G11" t="s">
         <v>16</v>
       </c>
       <c r="H11">
-        <v>550291</v>
+        <v>1264249</v>
       </c>
       <c r="I11" t="b">
         <v>0</v>
@@ -942,28 +1041,28 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
         <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="F12" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="G12" t="s">
         <v>16</v>
       </c>
       <c r="H12">
-        <v>448707</v>
+        <v>601792</v>
       </c>
       <c r="I12" t="b">
         <v>0</v>
@@ -974,28 +1073,28 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
         <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="F13" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="G13" t="s">
         <v>16</v>
       </c>
       <c r="H13">
-        <v>517334</v>
+        <v>731833</v>
       </c>
       <c r="I13" t="b">
         <v>0</v>
@@ -1006,28 +1105,28 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="F14" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="G14" t="s">
         <v>16</v>
       </c>
       <c r="H14">
-        <v>505959</v>
+        <v>559833</v>
       </c>
       <c r="I14" t="b">
         <v>0</v>
@@ -1038,28 +1137,28 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="D15" t="s">
         <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>14</v>
+        <v>68</v>
       </c>
       <c r="F15" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="G15" t="s">
         <v>16</v>
       </c>
       <c r="H15">
-        <v>483957</v>
+        <v>472708</v>
       </c>
       <c r="I15" t="b">
         <v>0</v>
@@ -1070,28 +1169,28 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="B16" t="s">
         <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
         <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="F16" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="G16" t="s">
         <v>16</v>
       </c>
       <c r="H16">
-        <v>398916</v>
+        <v>522374</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
@@ -1102,28 +1201,28 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="D17" t="s">
         <v>13</v>
       </c>
       <c r="E17" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="F17" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="G17" t="s">
         <v>16</v>
       </c>
       <c r="H17">
-        <v>386791</v>
+        <v>342082</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
@@ -1134,28 +1233,28 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="D18" t="s">
         <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="F18" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="G18" t="s">
         <v>16</v>
       </c>
       <c r="H18">
-        <v>362333</v>
+        <v>369166</v>
       </c>
       <c r="I18" t="b">
         <v>0</v>

</xml_diff>